<commit_message>
Display PB0 press on LCD display moved ext_ble_signal to ble.h updated Server Command Table Updated IRQ/events for GPIO for PB0
</commit_message>
<xml_diff>
--- a/questions/Server Command Table A8.xlsx
+++ b/questions/Server Command Table A8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment8-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EA33CD-773D-4D50-862C-F039791CB552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714BCAE8-CF02-46E4-9A7D-4C43AF04AC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="1740" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -152,6 +152,24 @@
   </si>
   <si>
     <t>sl_bt_sm_bonding_confirm()</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_delete_bondings()</t>
+  </si>
+  <si>
+    <t>Delete previous bondings per A8 spec</t>
+  </si>
+  <si>
+    <t>Update GATT characteristic, update display</t>
+  </si>
+  <si>
+    <t>Only for PB0 button presses (since it's not state machine)</t>
+  </si>
+  <si>
+    <t>updateAndDisplay_PB0gatt()</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_system_external_signal_id</t>
   </si>
 </sst>
 </file>
@@ -353,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,18 +453,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
@@ -456,6 +462,21 @@
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1619,10 +1640,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1639,13 +1660,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1718,15 +1739,19 @@
       <c r="B7" s="27"/>
       <c r="C7" s="31"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="30"/>
+      <c r="E7" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="41" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="12"/>
@@ -1736,7 +1761,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="36"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1744,7 +1769,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="36"/>
+      <c r="E10" s="41"/>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -1817,124 +1842,156 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="26"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="38" t="s">
-        <v>26</v>
-      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="25"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="C23" s="16"/>
       <c r="D23" s="25"/>
-      <c r="E23" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19"/>
-      <c r="B24" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="33"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="17"/>
+      <c r="B25" s="34" t="s">
+        <v>26</v>
+      </c>
       <c r="C25" s="16"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="25"/>
+    </row>
+    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="26" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="16"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="22"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="41" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="16"/>
+    </row>
+    <row r="29" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19"/>
+      <c r="B31" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="21"/>
+    </row>
+    <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Allow Bonding with client Modified excel file
</commit_message>
<xml_diff>
--- a/questions/Server Command Table A8.xlsx
+++ b/questions/Server Command Table A8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment8-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714BCAE8-CF02-46E4-9A7D-4C43AF04AC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B44E23-30D6-485A-820E-063FBE785E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="7395" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -170,6 +170,17 @@
   </si>
   <si>
     <t>sl_bt_evt_system_external_signal_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security  manager, </t>
+  </si>
+  <si>
+    <t>sl_bt_sm_configure()
+sl_bt_sm_set_bondable_mode()</t>
+  </si>
+  <si>
+    <t>waitForPB0Press()
+sl_bt_sm_passkey_confirm()</t>
   </si>
 </sst>
 </file>
@@ -462,6 +473,9 @@
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,9 +486,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1642,8 +1653,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B27" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1660,13 +1671,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1751,7 +1762,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="42" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="12"/>
@@ -1761,7 +1772,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1769,15 +1780,19 @@
       <c r="B10" s="4"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="41"/>
-    </row>
-    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="42"/>
+    </row>
+    <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
@@ -1867,7 +1882,7 @@
       <c r="B20" s="20"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="22" t="s">
@@ -1946,7 +1961,9 @@
       <c r="B28" s="17"/>
       <c r="C28" s="16"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="24"/>
+      <c r="E28" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="F28" s="16"/>
     </row>
     <row r="29" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update A8 excel sheet, added diagram, update comments and add bl_connection_set_parameters() for submission
</commit_message>
<xml_diff>
--- a/questions/Server Command Table A8.xlsx
+++ b/questions/Server Command Table A8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hyounjun\Desktop\CU_Boulder\ECEN5823\assignments\ecen5823_workspace\ecen5823-assignment8-hyounjunchang\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B44E23-30D6-485A-820E-063FBE785E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC29E764-0311-4212-ADD5-A3A43B1ADDB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="7395" windowWidth="24885" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>Client Command Table for A7</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Use this table to help you design your program. Add rows as needed.</t>
   </si>
@@ -95,23 +92,6 @@
     </r>
   </si>
   <si>
-    <t>Prevent charge build-up on LCD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This event indicates that a soft timer has expired. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>displayUpdate() - not a BLE function</t>
-    </r>
-  </si>
-  <si>
     <t>Events only for Slaves/Server</t>
   </si>
   <si>
@@ -129,58 +109,153 @@
     <t>Request Bluetooth Connection parameters to client, may be ignored by client</t>
   </si>
   <si>
-    <t>sl_bt_legacy_advertiser_generate_data()
+    <t>sl_bt_evt_gatt_server_characteristic_status_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_confirm_bonding_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_confirm_passkey_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_bonded_id</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_sm_bonding_failed_id</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_bonding_confirm()</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_delete_bondings()</t>
+  </si>
+  <si>
+    <t>Delete previous bondings per A8 spec</t>
+  </si>
+  <si>
+    <t>Only for PB0 button presses (since it's not state machine)</t>
+  </si>
+  <si>
+    <t>sl_bt_evt_system_external_signal_id</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_configure()</t>
+  </si>
+  <si>
+    <t>Security  manager, flag set to 0x2F</t>
+  </si>
+  <si>
+    <t>clear_flags_and_led()
+sl_bt_legacy_advertiser_generate_data()
 sl_bt_legacy_advertiser_start()</t>
   </si>
   <si>
-    <t>sl_bt_evt_gatt_server_characteristic_status_id</t>
-  </si>
-  <si>
-    <t>check_CCCD_change() or set_indication_received()</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_sm_confirm_bonding_id</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_sm_confirm_passkey_id</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_sm_bonded_id</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_sm_bonding_failed_id</t>
-  </si>
-  <si>
-    <t>sl_bt_sm_bonding_confirm()</t>
-  </si>
-  <si>
-    <t>sl_bt_sm_delete_bondings()</t>
-  </si>
-  <si>
-    <t>Delete previous bondings per A8 spec</t>
-  </si>
-  <si>
-    <t>Update GATT characteristic, update display</t>
-  </si>
-  <si>
-    <t>Only for PB0 button presses (since it's not state machine)</t>
-  </si>
-  <si>
-    <t>updateAndDisplay_PB0gatt()</t>
-  </si>
-  <si>
-    <t>sl_bt_evt_system_external_signal_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security  manager, </t>
-  </si>
-  <si>
-    <t>sl_bt_sm_configure()
-sl_bt_sm_set_bondable_mode()</t>
-  </si>
-  <si>
-    <t>waitForPB0Press()
-sl_bt_sm_passkey_confirm()</t>
+    <t>sl_bt_gatt_server_send_indication()
+displayUpdate() - not a BLE function</t>
+  </si>
+  <si>
+    <t>Send Indication is queue not empty
+Prevent charge build-up on LCD</t>
+  </si>
+  <si>
+    <t>update_PB0gatt()
+sl_bt_gatt_server_send_indication()</t>
+  </si>
+  <si>
+    <t>Update GATT characteristic, update display
+If indiation enabled</t>
+  </si>
+  <si>
+    <t>sl_bt_sm_passkey_confirm()</t>
+  </si>
+  <si>
+    <t>If checking passkey for bonding</t>
+  </si>
+  <si>
+    <t>Close all bondings on conenction disconnect</t>
+  </si>
+  <si>
+    <t>check_CCCD_change() or set_indication_received()
+gpioLEDsetOn/Off</t>
+  </si>
+  <si>
+    <t>If indication change, toggle LED0/LED1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+displayprintf()</t>
+  </si>
+  <si>
+    <t>Display the passkey</t>
+  </si>
+  <si>
+    <t>LOG_ERROR()
+sl_bt_connection_close()</t>
+  </si>
+  <si>
+    <t>Log Error and close connection</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Advertising"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Connected"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_9, "Button Released" or "Button Pressed"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Advertising"
+DISPLAY_ROW_9, "Button Released" or "Button Pressed"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_TEMP_VALUE, ""
+DISPLAY_ROW_PASSKEY, ""
+DISPLAY_ROW_ACTION, ""</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_TEMP_VALUE, temperature or ""</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_PASSKEY, passkey
+DISPLAY_ROW_ACTION, "Confirm with PB0"</t>
+  </si>
+  <si>
+    <t>DISPLAY_ROW_CONNECTION, "Bonded"
+DISPLAY_ROW_PASSKEY, ""
+DISPLAY_ROW_ACTION, ""</t>
+  </si>
+  <si>
+    <t>displayprintf()</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Update temperature state machine for all events not related to PB0</t>
+  </si>
+  <si>
+    <t>temperature_state_machine</t>
+  </si>
+  <si>
+    <t>BLE_LETIMER0_UF_FLAG
+BLE_LETIMER0_COMP1_FLAG
+BLE_I2C_TRANSFER_FLAG
+BLE_LETIMER0_COMP1_FLAG
+BLE_I2C_TRANSFER_FLAG</t>
+  </si>
+  <si>
+    <t>Server Command Table for A8</t>
+  </si>
+  <si>
+    <t>IDLE-&gt;WAIT_POWER_UP
+WAIT_POWER_UP-&gt;WAIT_I2C_WRITE
+WAIT_I2C_WRITE-&gt;WAIT_I2C_READ_START
+WAIT_I2C_READ_START-&gt;WAIT_I2C_READ_COMPLETE
+WAIT_I2C_READ_COMPLETE-&gt;IDLE</t>
+  </si>
+  <si>
+    <t>Doesn't affect SI7021 state machine, but necessary to set htm_indication to advance from Idle state</t>
   </si>
 </sst>
 </file>
@@ -273,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -378,11 +453,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -476,7 +564,14 @@
     <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -571,6 +666,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12555</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>513171</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>103691</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F84C15D-84BF-1E62-E50C-2C6D981463F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="15985247"/>
+          <a:ext cx="9064737" cy="4277949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1651,10 +1801,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B27" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1662,7 +1812,7 @@
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="74" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
@@ -1671,13 +1821,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
@@ -1690,40 +1840,40 @@
     <row r="3" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -1734,15 +1884,15 @@
     <row r="6" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="10"/>
       <c r="E6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,10 +1901,10 @@
       <c r="C7" s="31"/>
       <c r="D7" s="28"/>
       <c r="E7" s="29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1762,8 +1912,8 @@
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="42" t="s">
-        <v>20</v>
+      <c r="E8" s="45" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -1772,15 +1922,17 @@
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="42"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="40" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="42"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -1788,16 +1940,16 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1807,54 +1959,66 @@
     <row r="13" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="22"/>
+      <c r="C13" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="F14" s="16"/>
     </row>
     <row r="15" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="25"/>
       <c r="E15" s="16" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="16"/>
+      <c r="C16" s="25" t="s">
+        <v>46</v>
+      </c>
       <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="E16" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="24" t="s">
-        <v>18</v>
+      <c r="E17" s="39" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1868,147 +2032,197 @@
     <row r="19" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="37" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
       <c r="E19" s="36"/>
       <c r="F19" s="22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
+      <c r="C20" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="D20" s="21"/>
       <c r="E20" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="16"/>
-    </row>
-    <row r="24" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="26"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="41"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="34" t="s">
-        <v>26</v>
+      <c r="B25" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="25"/>
-      <c r="F25" s="25"/>
-    </row>
-    <row r="26" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="33"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="26"/>
+      <c r="C26" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="25"/>
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="16"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="19"/>
+      <c r="B29" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="25"/>
+      <c r="E30" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
+      <c r="C32" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="D32" s="22"/>
-      <c r="E32" s="36"/>
+      <c r="E32" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="F32" s="21"/>
     </row>
-    <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="25"/>
+    <row r="33" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2020,5 +2234,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>